<commit_message>
Fix 20 and sheet1
</commit_message>
<xml_diff>
--- a/data/instance/20/schedule_21.xlsx
+++ b/data/instance/20/schedule_21.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10212"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SCALE_Demo_toNCS\SCALE_Demo_toNCS\test_200304\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jianingju/Downloads/URECA/Project files/Bi-objective 2016 v1/data/instance/20/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D293EC0-F495-4350-83B7-EF809EEF290E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5042437B-2375-5B43-A99C-F2BEB4319E9C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="135" yWindow="390" windowWidth="16110" windowHeight="10320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="140" yWindow="500" windowWidth="16120" windowHeight="10320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="FlightSchedule" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -180,17 +180,17 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[hh]:mm:ss"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -229,7 +229,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -532,16 +532,16 @@
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="6" width="9" style="1"/>
     <col min="7" max="8" width="9" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -567,7 +567,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -593,7 +593,7 @@
         <v>4.0607629724433902</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -619,7 +619,7 @@
         <v>8.2259751195020403</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -645,7 +645,7 @@
         <v>4.5259667475579102</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -671,7 +671,7 @@
         <v>9.7467943448089596</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -697,7 +697,7 @@
         <v>3.2185982973959302</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -723,7 +723,7 @@
         <v>14.0801278403287</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -749,7 +749,7 @@
         <v>6.7627194973619797</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -775,7 +775,7 @@
         <v>13.44200505877</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -801,7 +801,7 @@
         <v>3.8405728739342999</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -827,7 +827,7 @@
         <v>4.9434299833212902</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -853,7 +853,7 @@
         <v>2.7838821814150099</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -879,7 +879,7 @@
         <v>4.4282473959795796</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -905,7 +905,7 @@
         <v>11.503622617824901</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -931,7 +931,7 @@
         <v>6.5192024052026403</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -957,7 +957,7 @@
         <v>6.0570207197928498</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -983,7 +983,7 @@
         <v>5.7973593126526097</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -1009,7 +1009,7 @@
         <v>19.367740575503301</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -1035,7 +1035,7 @@
         <v>7.9990233778880704</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -1061,7 +1061,7 @@
         <v>5.9358550352918797</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>20</v>
       </c>

</xml_diff>